<commit_message>
changes to prejudice remover and visualizations for final report
</commit_message>
<xml_diff>
--- a/visualizations/PrejRemSummary.xlsx
+++ b/visualizations/PrejRemSummary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johollen/recidivism/visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C53C5FB-06DF-2548-BF3D-37DAE75C6B88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D93CAA-D4C9-B14A-B43E-5E7ADF1B5014}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2440" windowWidth="32320" windowHeight="16440" xr2:uid="{D3952165-AEEC-2843-978A-C756F6019F28}"/>
+    <workbookView xWindow="1700" yWindow="860" windowWidth="32320" windowHeight="16440" xr2:uid="{D3952165-AEEC-2843-978A-C756F6019F28}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="old2" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,13 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>alpha</t>
-  </si>
-  <si>
-    <t>accuracy_advNN</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>average odds difference</t>
   </si>
@@ -52,6 +47,27 @@
   </si>
   <si>
     <t>disparate impact (-)</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>Eta</t>
+  </si>
+  <si>
+    <t>Disparate Impact</t>
+  </si>
+  <si>
+    <t>Average Odds Difference</t>
+  </si>
+  <si>
+    <t>Statistical Parity Difference</t>
+  </si>
+  <si>
+    <t>Equal Opportunity Difference</t>
+  </si>
+  <si>
+    <t>Balanced Accuracy</t>
   </si>
 </sst>
 </file>
@@ -87,8 +103,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,11 +158,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'old2'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>accuracy</c:v>
+                  <c:v>Balanced Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -153,7 +170,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -168,7 +185,7 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -176,48 +193,120 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'old2'!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>'old2'!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>64.8</c:v>
+                  <c:v>70.329999999999899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.099999999999994</c:v>
+                  <c:v>70.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.5</c:v>
+                  <c:v>69.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.4</c:v>
+                  <c:v>69.36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.1</c:v>
+                  <c:v>70.329999999999899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70.329999999999899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.329999999999899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.329999999999899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65.999999999999901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>63.23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>62.849999999999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61.970000000000006</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>61.829999999999899</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>61.659999999999904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -225,7 +314,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DE80-D344-A87D-2C1E0D1D1F01}"/>
+              <c16:uniqueId val="{00000000-CF0E-B246-8E5D-8E5C86B0D6E3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -248,11 +337,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'old2'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>disparate impact (-)</c:v>
+                  <c:v>Disparate Impact</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -275,7 +364,7 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -283,48 +372,120 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'old2'!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:f>'old2'!$C$2:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>-24.2</c:v>
+                  <c:v>-39.151059624108804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-20.6</c:v>
+                  <c:v>-37.634133182112699</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-16.2</c:v>
+                  <c:v>-35.325886260531398</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.12</c:v>
+                  <c:v>-30.312989306545603</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-39.151059624108804</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-39.151059624108804</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-39.151059624108804</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-39.151059624108804</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-12.2417887232663</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-13.075806869734199</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-6.9076215165262393</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-6.5338982501620197</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-11.4936795204147</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-11.2662524303305</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-11.0979131561892</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-11.1989322747893</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-11.183912832145101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,7 +493,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-DE80-D344-A87D-2C1E0D1D1F01}"/>
+              <c16:uniqueId val="{00000001-CF0E-B246-8E5D-8E5C86B0D6E3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -341,11 +502,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'old2'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>average odds difference</c:v>
+                  <c:v>Average Odds Difference</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -376,48 +537,120 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'old2'!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:f>'old2'!$D$2:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>-16</c:v>
+                  <c:v>-15.804102397926101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-14</c:v>
+                  <c:v>-15.236843810758199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-11</c:v>
+                  <c:v>-14.2659105638366</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>-12.323566104990199</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-15.804102397926101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-15.804102397926101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-15.804102397926101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-15.804102397926101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.47639338950097</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.6097488658457495</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.6636957226182703</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-7.5841979909267598</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-6.30914128321451</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-6.4693745949449095</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-6.5711276733635708</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-6.9392255346727101</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-7.0423509397277995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -425,7 +658,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-DE80-D344-A87D-2C1E0D1D1F01}"/>
+              <c16:uniqueId val="{00000002-CF0E-B246-8E5D-8E5C86B0D6E3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -434,11 +667,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>'old2'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>statistical parity difference</c:v>
+                  <c:v>Statistical Parity Difference</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -469,48 +702,120 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'old2'!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$6</c:f>
+              <c:f>'old2'!$E$2:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>-18</c:v>
+                  <c:v>-20.651339922229401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-15.4</c:v>
+                  <c:v>-20.100095593000599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-12.6</c:v>
+                  <c:v>-19.0953953337653</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>-17.129724562540499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-20.651339922229401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-20.651339922229401</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20.651339922229401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-20.651339922229401</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8.500831173039531</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-8.9228613091380407</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.3714727802981201</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.9646597537265</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-9.0031108230719301</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-8.9684769928710306</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-8.8778872326636389</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-9.0407501620220305</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-9.0540311082307205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,7 +823,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-DE80-D344-A87D-2C1E0D1D1F01}"/>
+              <c16:uniqueId val="{00000003-CF0E-B246-8E5D-8E5C86B0D6E3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -527,11 +832,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>'old2'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>equal opportunity difference</c:v>
+                  <c:v>Equal Opportunity Difference</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -562,48 +867,120 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'old2'!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$6</c:f>
+              <c:f>'old2'!$F$2:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>-9.8000000000000007</c:v>
+                  <c:v>-10.3950599481529</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8.6</c:v>
+                  <c:v>-9.7973460790667506</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.4</c:v>
+                  <c:v>-8.9312167854828211</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>-7.9004763447828905</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-10.3950599481529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10.3950599481529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-10.3950599481529</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10.3950599481529</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-4.0461697990926702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.3364938431626694</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.9921791963706998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-5.1791429034348599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.1981383668178802</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-3.9745998055735496</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-3.9745998055735496</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4.2188933895009706</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.2188933895009706</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -611,7 +988,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-DE80-D344-A87D-2C1E0D1D1F01}"/>
+              <c16:uniqueId val="{00000004-CF0E-B246-8E5D-8E5C86B0D6E3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -630,7 +1007,7 @@
         <c:axId val="710839919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.2"/>
+          <c:max val="200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -669,7 +1046,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1200" b="1"/>
-                  <a:t>alpha</a:t>
+                  <a:t>eta</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -748,6 +1125,8 @@
         <c:axId val="710841599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="72"/>
+          <c:min val="60"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -873,6 +1252,7 @@
         <c:axId val="725842543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -971,6 +1351,7 @@
         <c:crossAx val="725845551"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="725845551"/>
@@ -1003,8 +1384,1344 @@
           <c:yMode val="edge"/>
           <c:x val="2.3595800524934388E-2"/>
           <c:y val="0.81603450816049239"/>
-          <c:w val="0.9639195100612421"/>
-          <c:h val="0.18113589967920676"/>
+          <c:w val="0.96078043928719437"/>
+          <c:h val="0.18396556355051669"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13313670166229222"/>
+          <c:y val="5.5084060438391147E-2"/>
+          <c:w val="0.71475437445319334"/>
+          <c:h val="0.59672237955702523"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.68669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68579999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68389999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66490000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62849999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.62580000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.62879999999999903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.61470000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.61449999999999905</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.61429999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.61009999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.60919999999999896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DE80-D344-A87D-2C1E0D1D1F01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="710839919"/>
+        <c:axId val="710841599"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>disparate impact (-)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-0.428345317563188</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.41635053467271499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.37977595593000602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.428345317563188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.428345317563188</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.428345317563188</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.428345317563188</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20114269280622099</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.12771189241736799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.15576822747893701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.110398849643551</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.10175396953985701</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.10185964031108199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.104645998055735</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.10984136422553401</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.10402454633830201</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.10525899222294199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DE80-D344-A87D-2C1E0D1D1F01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>average odds difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-0.18955413156189199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.185480508749189</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.171833554763447</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.18955413156189199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.18955413156189199</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.18955413156189199</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.18955413156189199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.6126863253402403E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-6.3465181464679193E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-8.4293211276733601E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.2783003888528801E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-5.1225388852883899E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-5.49464841218405E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-5.7423622812702503E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-6.2147326636422501E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-5.8989436163318199E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6.0292206740116601E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DE80-D344-A87D-2C1E0D1D1F01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>statistical parity difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-0.224346046662346</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.22018732987686301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.20644711600777699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.224346046662346</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.224346046662346</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.224346046662346</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.224346046662346</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.127171727154893</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9.1402624756966894E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.110987167854828</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-8.0679082955281894E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-7.58253240440699E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.7180865197666801E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-7.9632615035644796E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-8.4076506804925399E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-8.0249724562540495E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-8.1278256642903404E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DE80-D344-A87D-2C1E0D1D1F01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>equal opportunity difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-0.16522106286454899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.16226579714841199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.14868188593648701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.16522106286454899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.16522106286454899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.16522106286454899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.16522106286454899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.110535839274141</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8.6645868438107496E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.9959850939727798E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-7.0922116007776995E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-6.9169880103694098E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-6.7116445236552094E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-7.1334656513285702E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-7.2823574206092007E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-7.2823574206092007E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-7.2823574206092007E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-DE80-D344-A87D-2C1E0D1D1F01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="725845551"/>
+        <c:axId val="725842543"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="710839919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1"/>
+                  <a:t>eta</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="710841599"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="710841599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Accuracy </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.9395669291338586E-2"/>
+              <c:y val="0.23746820109024833"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="710839919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="725842543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Fairness Metrics</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="725845551"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="725845551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="725842543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.3595800524934388E-2"/>
+          <c:y val="0.81603450816049239"/>
+          <c:w val="0.60920152559055119"/>
+          <c:h val="0.18396556355051669"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1120,6 +2837,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1636,20 +3393,579 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>692150</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA7396C6-B1E2-C141-9E14-3A6618757F35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1973,151 +4289,755 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3159C5F4-8C0A-9C4B-A215-7AE2909EB65E}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D6559CA-7848-854E-8F06-FA0758C89941}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:T15"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="6" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
+        <v>70.329999999999899</v>
+      </c>
+      <c r="C2">
+        <v>-39.151059624108804</v>
+      </c>
+      <c r="D2">
+        <v>-15.804102397926101</v>
+      </c>
+      <c r="E2">
+        <v>-20.651339922229401</v>
+      </c>
+      <c r="F2">
+        <v>-10.3950599481529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>70.3</v>
+      </c>
+      <c r="C3">
+        <v>-37.634133182112699</v>
+      </c>
+      <c r="D3">
+        <v>-15.236843810758199</v>
+      </c>
+      <c r="E3">
+        <v>-20.100095593000599</v>
+      </c>
+      <c r="F3">
+        <v>-9.7973460790667506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>69.97</v>
+      </c>
+      <c r="C4">
+        <v>-35.325886260531398</v>
+      </c>
+      <c r="D4">
+        <v>-14.2659105638366</v>
+      </c>
+      <c r="E4">
+        <v>-19.0953953337653</v>
+      </c>
+      <c r="F4">
+        <v>-8.9312167854828211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B5">
+        <v>69.36</v>
+      </c>
+      <c r="C5">
+        <v>-30.312989306545603</v>
+      </c>
+      <c r="D5">
+        <v>-12.323566104990199</v>
+      </c>
+      <c r="E5">
+        <v>-17.129724562540499</v>
+      </c>
+      <c r="F5">
+        <v>-7.9004763447828905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>70.329999999999899</v>
+      </c>
+      <c r="C6">
+        <v>-39.151059624108804</v>
+      </c>
+      <c r="D6">
+        <v>-15.804102397926101</v>
+      </c>
+      <c r="E6">
+        <v>-20.651339922229401</v>
+      </c>
+      <c r="F6">
+        <v>-10.3950599481529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>70.329999999999899</v>
+      </c>
+      <c r="C7">
+        <v>-39.151059624108804</v>
+      </c>
+      <c r="D7">
+        <v>-15.804102397926101</v>
+      </c>
+      <c r="E7">
+        <v>-20.651339922229401</v>
+      </c>
+      <c r="F7">
+        <v>-10.3950599481529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>70.329999999999899</v>
+      </c>
+      <c r="C8">
+        <v>-39.151059624108804</v>
+      </c>
+      <c r="D8">
+        <v>-15.804102397926101</v>
+      </c>
+      <c r="E8">
+        <v>-20.651339922229401</v>
+      </c>
+      <c r="F8">
+        <v>-10.3950599481529</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>70.329999999999899</v>
+      </c>
+      <c r="C9">
+        <v>-39.151059624108804</v>
+      </c>
+      <c r="D9">
+        <v>-15.804102397926101</v>
+      </c>
+      <c r="E9">
+        <v>-20.651339922229401</v>
+      </c>
+      <c r="F9">
+        <v>-10.3950599481529</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>65.999999999999901</v>
+      </c>
+      <c r="C10">
+        <v>-12.2417887232663</v>
+      </c>
+      <c r="D10">
+        <v>-5.47639338950097</v>
+      </c>
+      <c r="E10">
+        <v>-8.500831173039531</v>
+      </c>
+      <c r="F10">
+        <v>-4.0461697990926702</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>66.63</v>
+      </c>
+      <c r="C11">
+        <v>-13.075806869734199</v>
+      </c>
+      <c r="D11">
+        <v>-5.6097488658457495</v>
+      </c>
+      <c r="E11">
+        <v>-8.9228613091380407</v>
+      </c>
+      <c r="F11">
+        <v>-4.3364938431626694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>63.23</v>
+      </c>
+      <c r="C12">
+        <v>-6.9076215165262393</v>
+      </c>
+      <c r="D12">
+        <v>-3.6636957226182703</v>
+      </c>
+      <c r="E12">
+        <v>-5.3714727802981201</v>
+      </c>
+      <c r="F12">
+        <v>-2.9921791963706998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>75</v>
+      </c>
+      <c r="B13">
+        <v>63.2</v>
+      </c>
+      <c r="C13">
+        <v>-6.5338982501620197</v>
+      </c>
+      <c r="D13">
+        <v>-7.5841979909267598</v>
+      </c>
+      <c r="E13">
+        <v>-4.9646597537265</v>
+      </c>
+      <c r="F13">
+        <v>-5.1791429034348599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>62.849999999999994</v>
+      </c>
+      <c r="C14">
+        <v>-11.4936795204147</v>
+      </c>
+      <c r="D14">
+        <v>-6.30914128321451</v>
+      </c>
+      <c r="E14">
+        <v>-9.0031108230719301</v>
+      </c>
+      <c r="F14">
+        <v>-4.1981383668178802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>125</v>
+      </c>
+      <c r="B15">
+        <v>62.5</v>
+      </c>
+      <c r="C15">
+        <v>-11.2662524303305</v>
+      </c>
+      <c r="D15">
+        <v>-6.4693745949449095</v>
+      </c>
+      <c r="E15">
+        <v>-8.9684769928710306</v>
+      </c>
+      <c r="F15">
+        <v>-3.9745998055735496</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>150</v>
+      </c>
+      <c r="B16">
+        <v>61.970000000000006</v>
+      </c>
+      <c r="C16">
+        <v>-11.0979131561892</v>
+      </c>
+      <c r="D16">
+        <v>-6.5711276733635708</v>
+      </c>
+      <c r="E16">
+        <v>-8.8778872326636389</v>
+      </c>
+      <c r="F16">
+        <v>-3.9745998055735496</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>175</v>
+      </c>
+      <c r="B17">
+        <v>61.829999999999899</v>
+      </c>
+      <c r="C17">
+        <v>-11.1989322747893</v>
+      </c>
+      <c r="D17">
+        <v>-6.9392255346727101</v>
+      </c>
+      <c r="E17">
+        <v>-9.0407501620220305</v>
+      </c>
+      <c r="F17">
+        <v>-4.2188933895009706</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>200</v>
+      </c>
+      <c r="B18">
+        <v>61.659999999999904</v>
+      </c>
+      <c r="C18">
+        <v>-11.183912832145101</v>
+      </c>
+      <c r="D18">
+        <v>-7.0423509397277995</v>
+      </c>
+      <c r="E18">
+        <v>-9.0540311082307205</v>
+      </c>
+      <c r="F18">
+        <v>-4.2188933895009706</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3159C5F4-8C0A-9C4B-A215-7AE2909EB65E}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="6" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.68669999999999998</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-0.428345317563188</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-0.18955413156189199</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-0.224346046662346</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-0.16522106286454899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.68579999999999997</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-0.41635053467271499</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-0.185480508749189</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-0.22018732987686301</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-0.16226579714841199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
+      <c r="B4" s="1">
+        <v>0.68389999999999995</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-0.37977595593000602</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-0.171833554763447</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-0.20644711600777699</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-0.14868188593648701</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0.2</v>
-      </c>
-      <c r="B2">
-        <v>64.8</v>
-      </c>
-      <c r="C2">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="D2">
-        <v>-24.2</v>
-      </c>
-      <c r="E2">
-        <v>-16</v>
-      </c>
-      <c r="F2">
-        <v>-18</v>
-      </c>
-      <c r="G2">
-        <v>-9.8000000000000007</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.68669999999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-0.428345317563188</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-0.18955413156189199</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-0.224346046662346</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-0.16522106286454899</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>0.1</v>
-      </c>
-      <c r="B3">
-        <v>64.099999999999994</v>
-      </c>
-      <c r="C3">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="D3">
-        <v>-20.6</v>
-      </c>
-      <c r="E3">
-        <v>-14</v>
-      </c>
-      <c r="F3">
-        <v>-15.4</v>
-      </c>
-      <c r="G3">
-        <v>-8.6</v>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.68669999999999998</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-0.428345317563188</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-0.18955413156189199</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-0.224346046662346</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-0.16522106286454899</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>0.05</v>
-      </c>
-      <c r="B4">
-        <v>63.5</v>
-      </c>
-      <c r="C4">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="D4">
-        <v>-16.2</v>
-      </c>
-      <c r="E4">
-        <v>-11</v>
-      </c>
-      <c r="F4">
-        <v>-12.6</v>
-      </c>
-      <c r="G4">
-        <v>-6.4</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.68669999999999998</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-0.428345317563188</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-0.18955413156189199</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-0.224346046662346</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-0.16522106286454899</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>0.01</v>
-      </c>
-      <c r="B5">
-        <v>55.4</v>
-      </c>
-      <c r="C5">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="D5">
-        <v>-0.12</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.68669999999999998</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-0.428345317563188</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-0.18955413156189199</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-0.224346046662346</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-0.16522106286454899</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1E-3</v>
-      </c>
-      <c r="B6">
-        <v>55.1</v>
-      </c>
-      <c r="C6">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.66490000000000005</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-0.20114269280622099</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-9.6126863253402403E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-0.127171727154893</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-0.110535839274141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.62849999999999995</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-0.12771189241736799</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-6.3465181464679193E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-9.1402624756966894E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-8.6645868438107496E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.62580000000000002</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-0.15576822747893701</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-8.4293211276733601E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-0.110987167854828</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-9.9959850939727798E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.62879999999999903</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-0.110398849643551</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-5.2783003888528801E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-8.0679082955281894E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-7.0922116007776995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>75</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-0.10175396953985701</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-5.1225388852883899E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-7.58253240440699E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-6.9169880103694098E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.61470000000000002</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.10185964031108199</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-5.49464841218405E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-7.7180865197666801E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-6.7116445236552094E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>125</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.61449999999999905</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-0.104645998055735</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-5.7423622812702503E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-7.9632615035644796E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-7.1334656513285702E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>150</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.61429999999999996</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-0.10984136422553401</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-6.2147326636422501E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>-8.4076506804925399E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-7.2823574206092007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>175</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.61009999999999998</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-0.10402454633830201</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-5.8989436163318199E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>-8.0249724562540495E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-7.2823574206092007E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>200</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.60919999999999896</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-0.10525899222294199</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-6.0292206740116601E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>-8.1278256642903404E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-7.2823574206092007E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>